<commit_message>
Added ability to import comments and archived and fixed a null date of registration
</commit_message>
<xml_diff>
--- a/ImportToSRP3/template/CommunityListTemplate.xlsx
+++ b/ImportToSRP3/template/CommunityListTemplate.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18522"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\bahai\ImportToSRP3\ImportToSRP3\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{97B8A39C-54F4-4E7D-B72C-B855E678F2D2}" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Lookups" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AE$3</definedName>
+  </definedNames>
+  <calcPr calcId="171026"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="57">
   <si>
     <r>
       <t>First Name</t>
@@ -81,6 +85,9 @@
     <t>Estimated Age</t>
   </si>
   <si>
+    <t>Birth Date</t>
+  </si>
+  <si>
     <r>
       <t>Registered Bahai</t>
     </r>
@@ -140,6 +147,12 @@
     <t>Email</t>
   </si>
   <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Archived</t>
+  </si>
+  <si>
     <t>B1</t>
   </si>
   <si>
@@ -176,6 +189,9 @@
     <t>B10</t>
   </si>
   <si>
+    <t>Sample</t>
+  </si>
+  <si>
     <t>F</t>
   </si>
   <si>
@@ -185,68 +201,77 @@
     <t>Yes</t>
   </si>
   <si>
+    <t>SectorName</t>
+  </si>
+  <si>
+    <t>Neighborhood</t>
+  </si>
+  <si>
     <t>34 9th Avenue</t>
   </si>
   <si>
     <t xml:space="preserve">Alexandra </t>
   </si>
   <si>
+    <t>bbb@bbb.com</t>
+  </si>
+  <si>
+    <t>blah blah</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
+    <t>Badi</t>
+  </si>
+  <si>
+    <t>Kumar</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Leva</t>
+  </si>
+  <si>
+    <t>Midrand</t>
+  </si>
+  <si>
     <t>Age Category</t>
   </si>
   <si>
     <t>YesNo</t>
   </si>
   <si>
+    <t>MaleFemale</t>
+  </si>
+  <si>
+    <t>YN</t>
+  </si>
+  <si>
     <t>Junior Youth</t>
   </si>
   <si>
     <t>No</t>
   </si>
   <si>
+    <t>N</t>
+  </si>
+  <si>
     <t>Youth</t>
   </si>
   <si>
     <t>Child</t>
-  </si>
-  <si>
-    <t>MaleFemale</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>YN</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Sample</t>
-  </si>
-  <si>
-    <t>SectorName</t>
-  </si>
-  <si>
-    <t>Neighborhood</t>
-  </si>
-  <si>
-    <t>bbb@bbb.com</t>
-  </si>
-  <si>
-    <t>Birth Date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -664,36 +689,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AE3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.1796875" customWidth="1"/>
-    <col min="4" max="5" width="10.6328125" customWidth="1"/>
-    <col min="6" max="6" width="10.6328125" style="16" customWidth="1"/>
-    <col min="7" max="7" width="8.1796875" customWidth="1"/>
-    <col min="8" max="8" width="11.6328125" style="17" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" customWidth="1"/>
+    <col min="4" max="5" width="10.5703125" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="16" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" style="17" customWidth="1"/>
     <col min="9" max="10" width="11" customWidth="1"/>
-    <col min="11" max="11" width="35.1796875" customWidth="1"/>
-    <col min="12" max="12" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="35.140625" customWidth="1"/>
+    <col min="12" max="12" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.36328125" customWidth="1"/>
-    <col min="18" max="19" width="2.81640625" customWidth="1"/>
-    <col min="20" max="22" width="3.81640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="29" width="2.81640625" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="22.42578125" customWidth="1"/>
+    <col min="19" max="19" width="6.5703125" customWidth="1"/>
+    <col min="20" max="21" width="2.85546875" customWidth="1"/>
+    <col min="22" max="24" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="31" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" ht="22.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -710,112 +736,116 @@
         <v>4</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>49</v>
+        <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="R1" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="S1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:31" ht="15">
       <c r="A2" s="4" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="14">
         <v>29948</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H2" s="14">
-        <v>35490</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="H2" s="14"/>
       <c r="I2" s="6" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="M2" s="10">
         <v>2090</v>
@@ -824,73 +854,161 @@
       <c r="O2" s="7"/>
       <c r="P2" s="11"/>
       <c r="Q2" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="R2" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="R2" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="U2" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="V2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="W2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="X2" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA2" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE2" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" ht="15">
+      <c r="A3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="S2" s="10" t="s">
+      <c r="B3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="T2" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="U2" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="V2" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="W2" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="X2" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y2" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z2" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA2" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB2" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC2" s="10" t="s">
-        <v>43</v>
+      <c r="E3" s="6"/>
+      <c r="F3" s="14">
+        <v>29948</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="14">
+        <v>42768</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="M3" s="10">
+        <v>1684</v>
+      </c>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="R3" s="11"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="U3" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="V3" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="W3" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="X3" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y3" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z3" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA3" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB3" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC3" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD3" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE3" s="10" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="Q2" r:id="rId1"/>
+    <hyperlink ref="Q2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="Q3" r:id="rId2" xr:uid="{25004FDD-523B-4EA8-B108-3B0BA1FA4701}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>Lookups!$A$2:$A$5</xm:f>
           </x14:formula1>
           <xm:sqref>D2:D1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>Lookups!$D$2:$D$3</xm:f>
           </x14:formula1>
-          <xm:sqref>R2:AC1048576</xm:sqref>
+          <xm:sqref>T2:AE1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>Lookups!$C$2:$C$3</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
           <x14:formula1>
             <xm:f>Lookups!$B$2:$B$3</xm:f>
           </x14:formula1>
@@ -903,69 +1021,69 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6328125" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4">
       <c r="A1" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>42</v>
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" t="s">
-        <v>43</v>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" t="s">
-        <v>44</v>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>